<commit_message>
5.8 - update readme
</commit_message>
<xml_diff>
--- a/tietokanta/feats_class/feats_class.xlsx
+++ b/tietokanta/feats_class/feats_class.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Riku\Koulu\Ohjelmointyo\tietokanta\feats_class\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0E906C6-722C-4F40-888B-D6373D91094E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{604D5759-1A24-437B-919B-CD094BC4F170}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2625" yWindow="2625" windowWidth="21600" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="1920" windowWidth="21600" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>

</xml_diff>